<commit_message>
Revert "Revert "sentence tokenization""
This reverts commit 0d6e9847602ed3448fef181d28ee208cf3077ea3.
</commit_message>
<xml_diff>
--- a/data/positive_cleanup.xlsx
+++ b/data/positive_cleanup.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rsong_admin\Box Sync\classes\cs273\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workspace\cs273\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="668">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="664">
   <si>
     <t>trichloroethylene</t>
   </si>
@@ -716,9 +716,6 @@
     <t>copper hydroxide</t>
   </si>
   <si>
-    <t xml:space="preserve">copper </t>
-  </si>
-  <si>
     <t>potassium peroxide</t>
   </si>
   <si>
@@ -1079,9 +1076,6 @@
     <t>l-alanine</t>
   </si>
   <si>
-    <t>first, acetylene was treated with chlorine using a ferric chloride catalyst at 90 c to produce 1,1,2,2-tetrachloroethane according to the chemical equation the 1,1,2,2-tetrachloroethane is then dehydrochlorinated to give trichloroethylene.</t>
-  </si>
-  <si>
     <t>2-butanol is manufactured industrially by the hydration of 1-butene or 2-butene:  sulfuric acid is used as a catalyst for this conversion.</t>
   </si>
   <si>
@@ -1109,9 +1103,6 @@
     <t>cyclohexanone oxime can be prepared from the condensation reaction between cyclohexanone and hydroxylamine: alternatively, another industrial route involves the reaction of cyclohexane with nitrosyl c</t>
   </si>
   <si>
-    <t>the most famous and commercially important reaction of cyclohexanone oxime is its beckmann rearrangement yielding ??-caprolactam:  this reaction is catalyzed by sulfuric acid, but industrial scale reactions use solid acids.</t>
-  </si>
-  <si>
     <t>isopropylamine can be obtained by aminating isopropyl alcohol with ammonia in presence of a nickel/copper or similar catalyst</t>
   </si>
   <si>
@@ -1580,12 +1571,6 @@
     <t>the resulting potassium hydroxide is then carbonated using carbon dioxide to form potassium carbonate, which is often used to produce other potassium compounds.</t>
   </si>
   <si>
-    <t>hydrogen bromide and hydrobromic acid are important reagents in the production of inorganic and organic bromine compounds.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hydrogen bromide reacts with dichloromethane to give bromochloromethane and dibromomethane allyl bromide is prepared by treating allyl alcohol </t>
-  </si>
-  <si>
     <t xml:space="preserve">hydrogen bromide (along with hydrobromic acid) is produced by combining hydrogen and bromine at temperatures between </t>
   </si>
   <si>
@@ -1619,9 +1604,6 @@
     <t>sodium amide can be prepared by the reaction of sodium with ammonia gas, but it is usually prepared by the reaction in liquid ammonia using iron(iii) nitrate as a catalyst.</t>
   </si>
   <si>
-    <t>in the industrial production of indigo, sodium amide is a component of the highly basic mixture that induces cyclisation of n-phenylglycine.</t>
-  </si>
-  <si>
     <t>9,10-anthraquinone is obtained industrially by the oxidation of anthracene, a reaction that is localized at the central ring.</t>
   </si>
   <si>
@@ -1790,9 +1772,6 @@
     <t>potassium hydride is produced by direct combination of the metal and hydrogen: this reaction was discovered by humphry davy soon after his 1807 discovery of potassium, when he noted that the metal would vaporize in a cu</t>
   </si>
   <si>
-    <t>kh reacts with water according to the reaction: potassium hydride is a superbase that is stronger than sodium hydride.</t>
-  </si>
-  <si>
     <t>bromobenzene is an aryl halide, c6h5br, which can be formed by electrophilic aromatic substitution of benzene using bromine.</t>
   </si>
   <si>
@@ -2000,9 +1979,6 @@
     <t>in the laboratory, this compound may be prepared by reacting sodium cyanide with acetone, followed by acidification:  considering the high toxicity of acetone cyanohydrin</t>
   </si>
   <si>
-    <t>crushing the tubers releases these compounds and produces acetone cyanohydrin.</t>
-  </si>
-  <si>
     <t>today, industrial methanol is produced in a catalytic process directly from carbon monoxide, carbon dioxide, and hydrogen.</t>
   </si>
   <si>
@@ -2028,6 +2004,18 @@
   </si>
   <si>
     <t>enantiomerically pure (s)-2-chloropropionic acid is prepared from l-alanine via diazotization in hydrochloric acid.</t>
+  </si>
+  <si>
+    <t>first, acetylene was treated with chlorine using a ferric chloride catalyst at 90 c to produce 1,1,2,2-tetrachloroethane according to the chemical equation the 1,1,2,2-tetrachloroethane is then dehydrochlorinated to give trichloroethylene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">allyl bromide is prepared by treating allyl alcohol </t>
+  </si>
+  <si>
+    <t>2-chloroethanol</t>
+  </si>
+  <si>
+    <t>methyl methacrylate</t>
   </si>
 </sst>
 </file>
@@ -2364,10 +2352,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H267"/>
+  <dimension ref="A1:H269"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A229" workbookViewId="0">
+      <selection activeCell="D260" sqref="D260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2385,7 +2373,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>351</v>
+        <v>660</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2396,7 +2384,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2407,7 +2395,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2418,7 +2406,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2429,7 +2417,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2440,7 +2428,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2451,10 +2439,10 @@
         <v>13</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D7" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2465,7 +2453,7 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2476,10 +2464,7 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>360</v>
-      </c>
-      <c r="D9" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2490,7 +2475,7 @@
         <v>19</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -2501,13 +2486,13 @@
         <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="D11" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="E11" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2518,7 +2503,7 @@
         <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2529,7 +2514,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2540,10 +2525,10 @@
         <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="D14" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2554,10 +2539,10 @@
         <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="D15" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -2568,10 +2553,10 @@
         <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="D16" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2582,13 +2567,13 @@
         <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="D17" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="E17" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2607,7 +2592,7 @@
         <v>33</v>
       </c>
       <c r="C19" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -2618,7 +2603,7 @@
         <v>35</v>
       </c>
       <c r="C20" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2629,7 +2614,7 @@
         <v>31</v>
       </c>
       <c r="C21" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2640,7 +2625,7 @@
         <v>38</v>
       </c>
       <c r="C22" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -2651,10 +2636,10 @@
         <v>38</v>
       </c>
       <c r="C23" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="D23" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2665,7 +2650,7 @@
         <v>41</v>
       </c>
       <c r="C24" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2676,10 +2661,10 @@
         <v>43</v>
       </c>
       <c r="C25" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="D25" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -2690,7 +2675,7 @@
         <v>45</v>
       </c>
       <c r="C26" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -2717,7 +2702,7 @@
         <v>13</v>
       </c>
       <c r="C29" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -2728,7 +2713,7 @@
         <v>51</v>
       </c>
       <c r="C30" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -2739,10 +2724,10 @@
         <v>53</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D31" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -2753,7 +2738,7 @@
         <v>55</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -2764,10 +2749,10 @@
         <v>57</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -2778,16 +2763,16 @@
         <v>59</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="D34" t="s">
+        <v>392</v>
+      </c>
+      <c r="E34" t="s">
+        <v>393</v>
+      </c>
+      <c r="F34" t="s">
         <v>394</v>
-      </c>
-      <c r="D34" t="s">
-        <v>395</v>
-      </c>
-      <c r="E34" t="s">
-        <v>396</v>
-      </c>
-      <c r="F34" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -2798,7 +2783,7 @@
         <v>61</v>
       </c>
       <c r="C35" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -2809,7 +2794,7 @@
         <v>63</v>
       </c>
       <c r="C36" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -2820,22 +2805,22 @@
         <v>31</v>
       </c>
       <c r="C37" t="s">
+        <v>397</v>
+      </c>
+      <c r="D37" t="s">
+        <v>398</v>
+      </c>
+      <c r="E37" t="s">
+        <v>399</v>
+      </c>
+      <c r="F37" t="s">
         <v>400</v>
       </c>
-      <c r="D37" t="s">
+      <c r="G37" t="s">
         <v>401</v>
       </c>
-      <c r="E37" t="s">
+      <c r="H37" t="s">
         <v>402</v>
-      </c>
-      <c r="F37" t="s">
-        <v>403</v>
-      </c>
-      <c r="G37" t="s">
-        <v>404</v>
-      </c>
-      <c r="H37" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -2846,7 +2831,7 @@
         <v>51</v>
       </c>
       <c r="C38" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -2857,24 +2842,24 @@
         <v>66</v>
       </c>
       <c r="C39" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="D39" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="E39" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>65</v>
       </c>
       <c r="C40" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -2885,7 +2870,7 @@
         <v>68</v>
       </c>
       <c r="C41" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -2896,7 +2881,7 @@
         <v>67</v>
       </c>
       <c r="C42" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -2939,7 +2924,7 @@
         <v>75</v>
       </c>
       <c r="C47" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -2950,7 +2935,7 @@
         <v>77</v>
       </c>
       <c r="C48" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -2961,7 +2946,7 @@
         <v>27</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -2972,7 +2957,7 @@
         <v>27</v>
       </c>
       <c r="C50" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -2983,7 +2968,7 @@
         <v>80</v>
       </c>
       <c r="C51" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -2994,7 +2979,7 @@
         <v>31</v>
       </c>
       <c r="C52" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -3005,7 +2990,7 @@
         <v>48</v>
       </c>
       <c r="C53" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -3016,10 +3001,10 @@
         <v>84</v>
       </c>
       <c r="C54" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="D54" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -3030,7 +3015,7 @@
         <v>86</v>
       </c>
       <c r="C55" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -3041,10 +3026,10 @@
         <v>24</v>
       </c>
       <c r="C56" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="D56" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -3055,7 +3040,7 @@
         <v>89</v>
       </c>
       <c r="C57" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -3082,7 +3067,7 @@
         <v>48</v>
       </c>
       <c r="C60" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -3093,7 +3078,7 @@
         <v>95</v>
       </c>
       <c r="C61" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -3104,7 +3089,7 @@
         <v>97</v>
       </c>
       <c r="C62" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -3115,7 +3100,7 @@
         <v>97</v>
       </c>
       <c r="C63" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -3134,7 +3119,7 @@
         <v>51</v>
       </c>
       <c r="C65" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -3145,7 +3130,7 @@
         <v>102</v>
       </c>
       <c r="C66" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -3156,7 +3141,7 @@
         <v>51</v>
       </c>
       <c r="C67" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -3167,7 +3152,7 @@
         <v>13</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -3178,7 +3163,7 @@
         <v>106</v>
       </c>
       <c r="C69" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -3189,13 +3174,13 @@
         <v>97</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D70" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="E70" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -3214,7 +3199,7 @@
         <v>36</v>
       </c>
       <c r="C72" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -3225,7 +3210,7 @@
         <v>112</v>
       </c>
       <c r="C73" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -3236,7 +3221,7 @@
         <v>114</v>
       </c>
       <c r="C74" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -3247,7 +3232,7 @@
         <v>66</v>
       </c>
       <c r="C75" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -3274,7 +3259,7 @@
         <v>120</v>
       </c>
       <c r="C78" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -3285,7 +3270,7 @@
         <v>31</v>
       </c>
       <c r="C79" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -3296,7 +3281,7 @@
         <v>123</v>
       </c>
       <c r="C80" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -3307,10 +3292,10 @@
         <v>9</v>
       </c>
       <c r="C81" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="D81" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -3321,13 +3306,13 @@
         <v>126</v>
       </c>
       <c r="C82" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="D82" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="E82" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -3338,10 +3323,10 @@
         <v>19</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="D83" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -3352,7 +3337,7 @@
         <v>128</v>
       </c>
       <c r="C84" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -3363,7 +3348,7 @@
         <v>31</v>
       </c>
       <c r="C85" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -3374,7 +3359,7 @@
         <v>29</v>
       </c>
       <c r="C86" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -3385,10 +3370,10 @@
         <v>57</v>
       </c>
       <c r="C87" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="D87" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -3399,7 +3384,7 @@
         <v>133</v>
       </c>
       <c r="C88" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -3410,7 +3395,7 @@
         <v>135</v>
       </c>
       <c r="C89" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -3421,10 +3406,10 @@
         <v>137</v>
       </c>
       <c r="C90" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="D90" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -3435,7 +3420,7 @@
         <v>139</v>
       </c>
       <c r="C91" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -3446,13 +3431,13 @@
         <v>141</v>
       </c>
       <c r="C92" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="D92" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="E92" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -3463,7 +3448,7 @@
         <v>124</v>
       </c>
       <c r="C93" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -3474,7 +3459,7 @@
         <v>38</v>
       </c>
       <c r="C94" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -3485,7 +3470,7 @@
         <v>9</v>
       </c>
       <c r="C95" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -3496,7 +3481,7 @@
         <v>97</v>
       </c>
       <c r="C96" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -3507,7 +3492,7 @@
         <v>33</v>
       </c>
       <c r="C97" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -3518,10 +3503,10 @@
         <v>148</v>
       </c>
       <c r="C98" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D98" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -3532,7 +3517,7 @@
         <v>150</v>
       </c>
       <c r="C99" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -3543,10 +3528,10 @@
         <v>152</v>
       </c>
       <c r="C100" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="D100" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -3557,7 +3542,7 @@
         <v>38</v>
       </c>
       <c r="C101" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -3584,7 +3569,7 @@
         <v>74</v>
       </c>
       <c r="C104" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -3603,10 +3588,10 @@
         <v>19</v>
       </c>
       <c r="C106" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="D106" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -3617,7 +3602,7 @@
         <v>29</v>
       </c>
       <c r="C107" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -3628,7 +3613,7 @@
         <v>78</v>
       </c>
       <c r="C108" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -3639,10 +3624,10 @@
         <v>163</v>
       </c>
       <c r="C109" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="D109" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -3653,7 +3638,7 @@
         <v>9</v>
       </c>
       <c r="C110" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -3664,7 +3649,7 @@
         <v>108</v>
       </c>
       <c r="C111" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -3675,7 +3660,7 @@
         <v>167</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -3694,7 +3679,7 @@
         <v>49</v>
       </c>
       <c r="C114" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -3705,7 +3690,7 @@
         <v>171</v>
       </c>
       <c r="C115" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -3724,7 +3709,7 @@
         <v>175</v>
       </c>
       <c r="C117" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -3735,7 +3720,7 @@
         <v>177</v>
       </c>
       <c r="C118" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -3746,7 +3731,7 @@
         <v>179</v>
       </c>
       <c r="C119" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -3757,10 +3742,10 @@
         <v>97</v>
       </c>
       <c r="C120" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="D120" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -3771,7 +3756,7 @@
         <v>182</v>
       </c>
       <c r="C121" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -3790,7 +3775,7 @@
         <v>186</v>
       </c>
       <c r="C123" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -3809,7 +3794,7 @@
         <v>49</v>
       </c>
       <c r="C125" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -3836,7 +3821,7 @@
         <v>182</v>
       </c>
       <c r="C128" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -3855,7 +3840,7 @@
         <v>17</v>
       </c>
       <c r="C130" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -3866,7 +3851,7 @@
         <v>195</v>
       </c>
       <c r="C131" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -3877,7 +3862,7 @@
         <v>27</v>
       </c>
       <c r="C132" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
@@ -3888,7 +3873,7 @@
         <v>80</v>
       </c>
       <c r="C133" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
@@ -3899,10 +3884,10 @@
         <v>19</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="D134" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -3913,7 +3898,7 @@
         <v>15</v>
       </c>
       <c r="C135" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
@@ -3924,10 +3909,10 @@
         <v>199</v>
       </c>
       <c r="C136" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="D136" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -3938,7 +3923,7 @@
         <v>201</v>
       </c>
       <c r="C137" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -3949,7 +3934,7 @@
         <v>13</v>
       </c>
       <c r="C138" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -3960,13 +3945,13 @@
         <v>203</v>
       </c>
       <c r="C139" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="D139" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="E139" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
@@ -3977,13 +3962,13 @@
         <v>205</v>
       </c>
       <c r="C140" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="D140" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="E140" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
@@ -4002,7 +3987,7 @@
         <v>208</v>
       </c>
       <c r="C142" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
@@ -4013,7 +3998,7 @@
         <v>210</v>
       </c>
       <c r="C143" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
@@ -4024,10 +4009,10 @@
         <v>211</v>
       </c>
       <c r="C144" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>212</v>
       </c>
@@ -4035,19 +4020,16 @@
         <v>94</v>
       </c>
       <c r="C145" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="D145" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="E145" t="s">
-        <v>520</v>
-      </c>
-      <c r="F145" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>213</v>
       </c>
@@ -4055,10 +4037,10 @@
         <v>19</v>
       </c>
       <c r="C146" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>214</v>
       </c>
@@ -4066,10 +4048,10 @@
         <v>182</v>
       </c>
       <c r="C147" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>215</v>
       </c>
@@ -4077,10 +4059,10 @@
         <v>19</v>
       </c>
       <c r="C148" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>216</v>
       </c>
@@ -4088,10 +4070,10 @@
         <v>48</v>
       </c>
       <c r="C149" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>137</v>
       </c>
@@ -4099,13 +4081,13 @@
         <v>53</v>
       </c>
       <c r="C150" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="D150" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>217</v>
       </c>
@@ -4113,10 +4095,10 @@
         <v>218</v>
       </c>
       <c r="C151" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>219</v>
       </c>
@@ -4124,10 +4106,10 @@
         <v>220</v>
       </c>
       <c r="C152" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>221</v>
       </c>
@@ -4135,13 +4117,10 @@
         <v>42</v>
       </c>
       <c r="C153" t="s">
-        <v>530</v>
-      </c>
-      <c r="D153" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>222</v>
       </c>
@@ -4149,10 +4128,10 @@
         <v>223</v>
       </c>
       <c r="C154" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>224</v>
       </c>
@@ -4160,10 +4139,10 @@
         <v>225</v>
       </c>
       <c r="C155" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>226</v>
       </c>
@@ -4171,10 +4150,10 @@
         <v>227</v>
       </c>
       <c r="C156" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
         <v>228</v>
       </c>
@@ -4182,109 +4161,106 @@
         <v>45</v>
       </c>
       <c r="C157" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
         <v>229</v>
       </c>
       <c r="B158" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C158" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A159" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="C158" t="s">
-        <v>536</v>
-      </c>
-      <c r="D158" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A159" s="2" t="s">
+      <c r="B159" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="B159" s="2" t="s">
+      <c r="C159" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A160" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="C159" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A160" s="2" t="s">
+      <c r="B160" s="2" t="s">
         <v>233</v>
-      </c>
-      <c r="B160" s="2" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B161" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="B161" s="2" t="s">
-        <v>236</v>
-      </c>
       <c r="C161" t="s">
-        <v>538</v>
+        <v>532</v>
       </c>
       <c r="D161" t="s">
-        <v>539</v>
+        <v>533</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B162" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C162" t="s">
-        <v>540</v>
+        <v>534</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B163" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="B163" s="2" t="s">
-        <v>239</v>
-      </c>
       <c r="C163" t="s">
-        <v>541</v>
+        <v>535</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B164" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C164" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B165" s="2" t="s">
         <v>43</v>
       </c>
       <c r="C165" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B166" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="B166" s="2" t="s">
-        <v>243</v>
-      </c>
       <c r="C166" t="s">
-        <v>544</v>
+        <v>538</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -4295,40 +4271,40 @@
         <v>38</v>
       </c>
       <c r="C167" t="s">
-        <v>545</v>
+        <v>539</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B168" s="2" t="s">
         <v>80</v>
       </c>
       <c r="C168" t="s">
-        <v>546</v>
+        <v>540</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B169" s="2" t="s">
         <v>43</v>
       </c>
       <c r="C169" t="s">
-        <v>547</v>
+        <v>541</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B170" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C170" t="s">
-        <v>548</v>
+        <v>542</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -4336,65 +4312,65 @@
         <v>45</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C171" t="s">
-        <v>549</v>
+        <v>543</v>
       </c>
       <c r="D171" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B172" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C172" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B173" s="2" t="s">
         <v>78</v>
       </c>
       <c r="C173" t="s">
-        <v>552</v>
+        <v>546</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B174" s="2" t="s">
         <v>218</v>
       </c>
       <c r="C174" t="s">
-        <v>553</v>
+        <v>547</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B175" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="B175" s="2" t="s">
-        <v>252</v>
-      </c>
       <c r="C175" s="1" t="s">
-        <v>554</v>
+        <v>548</v>
       </c>
       <c r="D175" t="s">
-        <v>555</v>
+        <v>549</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B176" s="2" t="s">
         <v>208</v>
@@ -4402,13 +4378,13 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B177" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C177" t="s">
-        <v>556</v>
+        <v>550</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
@@ -4419,73 +4395,73 @@
         <v>172</v>
       </c>
       <c r="C178" t="s">
-        <v>557</v>
+        <v>551</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B179" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C179" t="s">
-        <v>558</v>
+        <v>552</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B180" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C180" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B181" s="2" t="s">
         <v>133</v>
       </c>
       <c r="C181" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B182" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="B182" s="2" t="s">
-        <v>259</v>
-      </c>
       <c r="C182" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B183" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="B183" s="2" t="s">
-        <v>261</v>
-      </c>
       <c r="C183" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B184" s="2" t="s">
         <v>120</v>
       </c>
       <c r="C184" t="s">
-        <v>563</v>
+        <v>557</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
@@ -4493,24 +4469,24 @@
         <v>59</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C185" t="s">
-        <v>564</v>
+        <v>558</v>
       </c>
       <c r="D185" t="s">
-        <v>565</v>
+        <v>559</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B186" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C186" t="s">
-        <v>566</v>
+        <v>560</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
@@ -4518,87 +4494,87 @@
         <v>51</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C187" t="s">
-        <v>567</v>
+        <v>561</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B188" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C188" t="s">
-        <v>568</v>
+        <v>562</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="B189" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="B189" s="2" t="s">
-        <v>268</v>
-      </c>
       <c r="C189" t="s">
-        <v>569</v>
+        <v>563</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B190" s="2" t="s">
         <v>177</v>
       </c>
       <c r="C190" t="s">
-        <v>570</v>
+        <v>564</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B191" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="B191" s="2" t="s">
-        <v>271</v>
-      </c>
       <c r="C191" t="s">
-        <v>571</v>
+        <v>565</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B192" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="B192" s="2" t="s">
-        <v>273</v>
-      </c>
       <c r="C192" t="s">
-        <v>571</v>
+        <v>565</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B193" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="B193" s="2" t="s">
-        <v>275</v>
-      </c>
       <c r="C193" s="1" t="s">
-        <v>573</v>
+        <v>567</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B194" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="B194" s="2" t="s">
-        <v>277</v>
-      </c>
       <c r="C194" t="s">
-        <v>572</v>
+        <v>566</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
@@ -4609,7 +4585,7 @@
         <v>31</v>
       </c>
       <c r="C195" t="s">
-        <v>574</v>
+        <v>568</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
@@ -4625,26 +4601,26 @@
         <v>141</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C197" t="s">
-        <v>575</v>
+        <v>569</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B198" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="B198" s="2" t="s">
-        <v>280</v>
-      </c>
       <c r="C198" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B199" s="2" t="s">
         <v>196</v>
@@ -4658,12 +4634,12 @@
         <v>13</v>
       </c>
       <c r="C200" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B201" s="2" t="s">
         <v>126</v>
@@ -4677,7 +4653,7 @@
         <v>128</v>
       </c>
       <c r="C202" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -4688,10 +4664,10 @@
         <v>80</v>
       </c>
       <c r="C203" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
       <c r="D203" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
@@ -4702,125 +4678,122 @@
         <v>24</v>
       </c>
       <c r="C204" t="s">
-        <v>581</v>
+        <v>575</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C205" t="s">
-        <v>582</v>
+        <v>576</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B206" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C206" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B207" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C207" t="s">
-        <v>584</v>
+        <v>578</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B208" s="2" t="s">
         <v>285</v>
-      </c>
-      <c r="B208" s="2" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B209" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C209" t="s">
-        <v>585</v>
+        <v>579</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B210" s="2" t="s">
         <v>155</v>
       </c>
       <c r="C210" t="s">
-        <v>586</v>
+        <v>580</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C211" t="s">
-        <v>587</v>
-      </c>
-      <c r="D211" t="s">
-        <v>588</v>
+        <v>581</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B212" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C212" t="s">
-        <v>589</v>
+        <v>582</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B213" s="2" t="s">
         <v>182</v>
       </c>
       <c r="C213" t="s">
-        <v>590</v>
+        <v>583</v>
       </c>
       <c r="D213" t="s">
-        <v>591</v>
+        <v>584</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B214" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B214" s="2" t="s">
-        <v>292</v>
-      </c>
       <c r="C214" t="s">
-        <v>592</v>
+        <v>585</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B215" s="2" t="s">
         <v>38</v>
@@ -4828,198 +4801,198 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B216" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C216" t="s">
-        <v>593</v>
+        <v>586</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B217" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C217" t="s">
-        <v>594</v>
+        <v>587</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="B218" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="B218" s="2" t="s">
-        <v>297</v>
-      </c>
       <c r="C218" t="s">
-        <v>595</v>
+        <v>588</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B219" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="B219" s="2" t="s">
-        <v>299</v>
-      </c>
       <c r="C219" t="s">
-        <v>596</v>
+        <v>589</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B220" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C220" t="s">
-        <v>597</v>
+        <v>590</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B221" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="B221" s="2" t="s">
-        <v>302</v>
-      </c>
       <c r="C221" t="s">
-        <v>598</v>
+        <v>591</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B222" s="2" t="s">
         <v>202</v>
       </c>
       <c r="C222" t="s">
-        <v>599</v>
+        <v>592</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B223" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="B223" s="2" t="s">
-        <v>305</v>
-      </c>
       <c r="C223" t="s">
-        <v>600</v>
+        <v>593</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B224" s="2" t="s">
         <v>218</v>
       </c>
       <c r="C224" t="s">
-        <v>601</v>
+        <v>594</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C225" t="s">
-        <v>602</v>
+        <v>595</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="B226" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="B226" s="2" t="s">
-        <v>308</v>
-      </c>
       <c r="C226" t="s">
-        <v>603</v>
+        <v>596</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B227" s="2" t="s">
         <v>173</v>
       </c>
       <c r="C227" t="s">
-        <v>604</v>
+        <v>597</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B228" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C228" t="s">
-        <v>605</v>
+        <v>598</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B229" s="2" t="s">
         <v>100</v>
       </c>
       <c r="C229" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B230" s="2" t="s">
         <v>148</v>
       </c>
       <c r="C230" t="s">
-        <v>607</v>
+        <v>600</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B231" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C231" t="s">
-        <v>608</v>
+        <v>601</v>
       </c>
       <c r="D231" t="s">
-        <v>609</v>
+        <v>602</v>
       </c>
       <c r="E231" t="s">
-        <v>610</v>
+        <v>603</v>
       </c>
       <c r="F231" t="s">
-        <v>611</v>
+        <v>604</v>
       </c>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B232" s="2" t="s">
         <v>97</v>
       </c>
       <c r="C232" t="s">
-        <v>612</v>
+        <v>605</v>
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.25">
@@ -5030,27 +5003,27 @@
         <v>38</v>
       </c>
       <c r="C233" t="s">
-        <v>613</v>
+        <v>606</v>
       </c>
       <c r="D233" t="s">
-        <v>614</v>
+        <v>607</v>
       </c>
       <c r="E233" t="s">
-        <v>615</v>
+        <v>608</v>
       </c>
       <c r="F233" t="s">
-        <v>616</v>
+        <v>609</v>
       </c>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B234" s="2" t="s">
         <v>95</v>
       </c>
       <c r="C234" t="s">
-        <v>617</v>
+        <v>610</v>
       </c>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.25">
@@ -5061,410 +5034,423 @@
         <v>31</v>
       </c>
       <c r="C235" t="s">
-        <v>618</v>
-      </c>
-      <c r="D235" t="s">
-        <v>619</v>
+        <v>611</v>
       </c>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236" s="2" t="s">
-        <v>315</v>
+        <v>33</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>316</v>
+        <v>662</v>
       </c>
       <c r="C236" t="s">
-        <v>620</v>
+        <v>612</v>
       </c>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>53</v>
+        <v>315</v>
       </c>
       <c r="C237" t="s">
-        <v>621</v>
+        <v>613</v>
       </c>
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238" s="2" t="s">
-        <v>302</v>
+        <v>316</v>
       </c>
       <c r="B238" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C238" t="s">
-        <v>622</v>
+        <v>614</v>
       </c>
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239" s="2" t="s">
-        <v>318</v>
+        <v>301</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>319</v>
+        <v>53</v>
       </c>
       <c r="C239" t="s">
-        <v>623</v>
+        <v>615</v>
       </c>
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>285</v>
+        <v>318</v>
       </c>
       <c r="C240" t="s">
-        <v>624</v>
+        <v>616</v>
       </c>
     </row>
     <row r="241" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B241" s="2" t="s">
-        <v>51</v>
+        <v>284</v>
+      </c>
+      <c r="C241" t="s">
+        <v>617</v>
       </c>
     </row>
     <row r="242" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A242" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>322</v>
+        <v>51</v>
       </c>
     </row>
     <row r="243" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C243" t="s">
-        <v>625</v>
+        <v>321</v>
       </c>
     </row>
     <row r="244" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>325</v>
+        <v>13</v>
       </c>
       <c r="C244" t="s">
-        <v>626</v>
+        <v>618</v>
       </c>
     </row>
     <row r="245" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A245" s="2" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B245" s="2" t="s">
-        <v>182</v>
+        <v>324</v>
       </c>
       <c r="C245" t="s">
-        <v>627</v>
-      </c>
-      <c r="D245" t="s">
-        <v>628</v>
+        <v>619</v>
       </c>
     </row>
     <row r="246" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>292</v>
+        <v>182</v>
       </c>
       <c r="C246" t="s">
-        <v>629</v>
+        <v>620</v>
       </c>
       <c r="D246" t="s">
-        <v>630</v>
+        <v>621</v>
       </c>
     </row>
     <row r="247" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>205</v>
+        <v>291</v>
       </c>
       <c r="C247" t="s">
-        <v>631</v>
+        <v>622</v>
+      </c>
+      <c r="D247" t="s">
+        <v>623</v>
       </c>
     </row>
     <row r="248" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>330</v>
+        <v>205</v>
       </c>
       <c r="C248" t="s">
-        <v>632</v>
+        <v>624</v>
       </c>
     </row>
     <row r="249" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A249" s="2" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>317</v>
+        <v>329</v>
       </c>
       <c r="C249" t="s">
-        <v>633</v>
+        <v>625</v>
       </c>
     </row>
     <row r="250" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A250" s="2" t="s">
-        <v>182</v>
+        <v>330</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>302</v>
+        <v>316</v>
       </c>
       <c r="C250" t="s">
-        <v>634</v>
-      </c>
-      <c r="D250" t="s">
-        <v>635</v>
+        <v>626</v>
       </c>
     </row>
     <row r="251" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A251" s="2" t="s">
-        <v>80</v>
+        <v>182</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>38</v>
+        <v>301</v>
       </c>
       <c r="C251" t="s">
-        <v>636</v>
+        <v>627</v>
       </c>
       <c r="D251" t="s">
-        <v>637</v>
-      </c>
-      <c r="E251" t="s">
-        <v>638</v>
-      </c>
-      <c r="F251" t="s">
-        <v>639</v>
-      </c>
-      <c r="G251" t="s">
-        <v>640</v>
-      </c>
-      <c r="H251" t="s">
-        <v>641</v>
+        <v>628</v>
       </c>
     </row>
     <row r="252" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A252" s="2" t="s">
-        <v>332</v>
+        <v>80</v>
       </c>
       <c r="B252" s="2" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
       <c r="C252" t="s">
-        <v>642</v>
+        <v>629</v>
       </c>
       <c r="D252" t="s">
-        <v>643</v>
+        <v>630</v>
+      </c>
+      <c r="E252" t="s">
+        <v>631</v>
+      </c>
+      <c r="F252" t="s">
+        <v>632</v>
+      </c>
+      <c r="G252" t="s">
+        <v>633</v>
+      </c>
+      <c r="H252" t="s">
+        <v>634</v>
       </c>
     </row>
     <row r="253" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A253" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>334</v>
+        <v>97</v>
       </c>
       <c r="C253" t="s">
-        <v>644</v>
+        <v>635</v>
       </c>
       <c r="D253" t="s">
-        <v>645</v>
+        <v>636</v>
       </c>
     </row>
     <row r="254" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="B254" s="2" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C254" t="s">
-        <v>646</v>
+        <v>637</v>
+      </c>
+      <c r="D254" t="s">
+        <v>638</v>
       </c>
     </row>
     <row r="255" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B255" s="2" t="s">
-        <v>186</v>
+        <v>335</v>
       </c>
       <c r="C255" t="s">
-        <v>647</v>
-      </c>
-      <c r="D255" t="s">
-        <v>648</v>
+        <v>639</v>
       </c>
     </row>
     <row r="256" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B256" s="2" t="s">
-        <v>339</v>
+        <v>186</v>
       </c>
       <c r="C256" t="s">
-        <v>649</v>
+        <v>640</v>
+      </c>
+      <c r="D256" t="s">
+        <v>641</v>
       </c>
     </row>
     <row r="257" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A257" s="2" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B257" s="2" t="s">
-        <v>9</v>
+        <v>338</v>
       </c>
       <c r="C257" t="s">
-        <v>650</v>
-      </c>
-      <c r="D257" t="s">
-        <v>651</v>
-      </c>
-      <c r="E257" t="s">
-        <v>652</v>
+        <v>642</v>
       </c>
     </row>
     <row r="258" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>342</v>
+        <v>9</v>
       </c>
       <c r="C258" t="s">
-        <v>653</v>
+        <v>643</v>
       </c>
       <c r="D258" t="s">
-        <v>654</v>
+        <v>644</v>
+      </c>
+      <c r="E258" t="s">
+        <v>645</v>
       </c>
     </row>
     <row r="259" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>52</v>
+        <v>341</v>
       </c>
       <c r="C259" t="s">
-        <v>655</v>
+        <v>646</v>
       </c>
       <c r="D259" t="s">
-        <v>656</v>
-      </c>
-      <c r="E259" t="s">
-        <v>657</v>
-      </c>
-      <c r="F259" t="s">
-        <v>658</v>
+        <v>647</v>
       </c>
     </row>
     <row r="260" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
-        <v>38</v>
+        <v>342</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>227</v>
+        <v>52</v>
       </c>
       <c r="C260" t="s">
-        <v>659</v>
-      </c>
-      <c r="D260" t="s">
-        <v>660</v>
-      </c>
-      <c r="E260" t="s">
-        <v>661</v>
-      </c>
-      <c r="F260" t="s">
-        <v>662</v>
+        <v>650</v>
       </c>
     </row>
     <row r="261" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A261" s="2" t="s">
-        <v>344</v>
+        <v>663</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>208</v>
+        <v>342</v>
+      </c>
+      <c r="C261" t="s">
+        <v>648</v>
+      </c>
+      <c r="D261" t="s">
+        <v>649</v>
       </c>
     </row>
     <row r="262" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A262" s="2" t="s">
-        <v>247</v>
+        <v>38</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>53</v>
+        <v>227</v>
       </c>
       <c r="C262" t="s">
-        <v>663</v>
+        <v>651</v>
+      </c>
+      <c r="D262" t="s">
+        <v>652</v>
+      </c>
+      <c r="E262" t="s">
+        <v>653</v>
+      </c>
+      <c r="F262" t="s">
+        <v>654</v>
       </c>
     </row>
     <row r="263" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C263" t="s">
-        <v>664</v>
+        <v>208</v>
       </c>
     </row>
     <row r="264" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
-        <v>263</v>
+        <v>246</v>
       </c>
       <c r="B264" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C264" t="s">
-        <v>665</v>
+        <v>655</v>
       </c>
     </row>
     <row r="265" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B265" s="2" t="s">
-        <v>347</v>
+        <v>116</v>
+      </c>
+      <c r="C265" t="s">
+        <v>656</v>
       </c>
     </row>
     <row r="266" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A266" s="2" t="s">
-        <v>348</v>
+        <v>262</v>
       </c>
       <c r="B266" s="2" t="s">
-        <v>139</v>
+        <v>51</v>
       </c>
       <c r="C266" t="s">
-        <v>666</v>
+        <v>657</v>
       </c>
     </row>
     <row r="267" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A267" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="B267" s="2" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A268" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="B268" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C268" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A269" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B269" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="B267" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="C267" t="s">
-        <v>667</v>
+      <c r="C269" t="s">
+        <v>659</v>
       </c>
     </row>
   </sheetData>

</xml_diff>